<commit_message>
Implemented most BitBoard::mask<> explicit template specializations. Still need a few more and test.
</commit_message>
<xml_diff>
--- a/forge/performance_log.xlsx
+++ b/forge/performance_log.xlsx
@@ -15,13 +15,14 @@
     <sheet name="Sheet12" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet6" sheetId="7" r:id="rId7"/>
     <sheet name="Sheet2" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet3" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="1979979923456" concurrentCalc="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="16">
   <si>
     <t xml:space="preserve">Solver Name</t>
   </si>
@@ -63,6 +64,12 @@
   </si>
   <si>
     <t xml:space="preserve">ApplePieHeuristic</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>???</t>
   </si>
 </sst>
 </file>
@@ -4422,4 +4429,166 @@
     </row>
   </sheetData>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E10"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>206603</v>
+      </c>
+      <c r="B5">
+        <v>158916.1875</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>3.07674503326416</v>
+      </c>
+      <c r="E5">
+        <v>1.30007517337799</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>189903</v>
+      </c>
+      <c r="B6">
+        <v>176677.578125</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>3.72142815589905</v>
+      </c>
+      <c r="E6">
+        <v>1.07485604286194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>190889</v>
+      </c>
+      <c r="B7">
+        <v>187163.359375</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>3.92193078994751</v>
+      </c>
+      <c r="E7">
+        <v>1.01990568637848</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>228744</v>
+      </c>
+      <c r="B8">
+        <v>17920.630859375</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>0.313374429941177</v>
+      </c>
+      <c r="E8">
+        <v>12.7642831802368</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>214282</v>
+      </c>
+      <c r="B9">
+        <v>187889.625</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>3.50733399391174</v>
+      </c>
+      <c r="E9">
+        <v>1.14046728610992</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>217141</v>
+      </c>
+      <c r="B10">
+        <v>194081.03125</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>3.57520771026611</v>
+      </c>
+      <c r="E10">
+        <v>1.11881613731384</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>